<commit_message>
changed : rename preview file and md file, move md jsonjs in db
</commit_message>
<xml_diff>
--- a/public/data/db_source/doc.xlsx
+++ b/public/data/db_source/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAD7051-3B66-A540-BEF9-9A188E9CDA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5FA82A-A4A2-EA40-91BE-3FD95963A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,18 +43,9 @@
     <t>data/pdf/pdf_wiki.pdf</t>
   </si>
   <si>
-    <t>folder_1_md</t>
-  </si>
-  <si>
     <t>md</t>
   </si>
   <si>
-    <t>example_1</t>
-  </si>
-  <si>
-    <t>data/md/folder/example_1.md</t>
-  </si>
-  <si>
     <t>pdf_online</t>
   </si>
   <si>
@@ -101,6 +92,15 @@
   </si>
   <si>
     <t>Communiqué de presse population</t>
+  </si>
+  <si>
+    <t>tourisme_exemple</t>
+  </si>
+  <si>
+    <t>Tourisme exemple</t>
+  </si>
+  <si>
+    <t>data/md/tourisme_exemple.md</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -507,16 +507,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>1716231182</v>
@@ -524,30 +524,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>1706212962</v>
@@ -555,16 +555,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>1606212962</v>
@@ -572,16 +572,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>1606212963</v>
@@ -589,16 +589,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>1724323867</v>

</xml_diff>

<commit_message>
fixed : jsonjsdb dont update last modification when no change
</commit_message>
<xml_diff>
--- a/public/data/db_source/doc.xlsx
+++ b/public/data/db_source/doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5FA82A-A4A2-EA40-91BE-3FD95963A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DAB01A-1414-334E-B051-E76F6C948996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>1706212962</v>
+        <v>1706219962</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added : doc description data
</commit_message>
<xml_diff>
--- a/public/data/db_source/doc.xlsx
+++ b/public/data/db_source/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DAB01A-1414-334E-B051-E76F6C948996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49145501-9ABE-6B4E-810A-019DDC232363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>data/md/tourisme_exemple.md</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>pdf wiki</t>
   </si>
 </sst>
 </file>
@@ -156,12 +162,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D411DE4-F6CC-B34F-83DD-A8AB904C9840}" name="Tableau1" displayName="Tableau1" ref="A1:E8" totalsRowShown="0">
-  <autoFilter ref="A1:E8" xr:uid="{9D411DE4-F6CC-B34F-83DD-A8AB904C9840}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9D411DE4-F6CC-B34F-83DD-A8AB904C9840}" name="Tableau1" displayName="Tableau1" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8" xr:uid="{9D411DE4-F6CC-B34F-83DD-A8AB904C9840}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{489DE2DA-302F-DA4C-B2C4-ED5D7CCA16C6}" name="id"/>
     <tableColumn id="6" xr3:uid="{1BC375FE-B2C2-D54F-8575-70DFED462C1B}" name="type"/>
     <tableColumn id="7" xr3:uid="{7626780A-ABC9-9346-A843-30F13339AED4}" name="name"/>
+    <tableColumn id="3" xr3:uid="{315CC133-1137-B448-B1D5-C08C4F4CF595}" name="description"/>
     <tableColumn id="8" xr3:uid="{7C4B401D-5858-8C42-969A-58DDE1F05BFC}" name="path"/>
     <tableColumn id="2" xr3:uid="{302DB002-0FC2-BD49-8544-1415D37BE0F0}" name="last_update"/>
   </tableColumns>
@@ -456,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -467,11 +474,12 @@
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,13 +490,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -499,13 +510,16 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1716215962</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -516,13 +530,16 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1716231182</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -533,10 +550,13 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -547,13 +567,16 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1706219962</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -564,13 +587,16 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1606212962</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -581,13 +607,16 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1606212963</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -598,9 +627,12 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1724323867</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed : jsonjsdb_editor prevent adding entry when old and new value are both null or empty
</commit_message>
<xml_diff>
--- a/public/data/db_source/doc.xlsx
+++ b/public/data/db_source/doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3125C24F-172A-4548-B774-EA867542D098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BDBB25-B514-BD42-A29F-01F193C40DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>